<commit_message>
conversion of "fa"-"fo" added
</commit_message>
<xml_diff>
--- a/state.xlsx
+++ b/state.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="164">
   <si>
     <t>state</t>
   </si>
@@ -106,6 +106,9 @@
     <t>w</t>
   </si>
   <si>
+    <t>f</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -491,6 +494,18 @@
   </si>
   <si>
     <t>ツォ</t>
+  </si>
+  <si>
+    <t>ファ</t>
+  </si>
+  <si>
+    <t>フィ</t>
+  </si>
+  <si>
+    <t>フェ</t>
+  </si>
+  <si>
+    <t>フォ</t>
   </si>
 </sst>
 </file>
@@ -512,28 +527,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -542,72 +535,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Yu Gothic"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Yu Gothic"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Yu Gothic"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -635,7 +567,91 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Yu Gothic"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Yu Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Yu Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -648,9 +664,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Yu Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -665,7 +680,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -677,19 +716,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,37 +734,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,19 +758,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,73 +854,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,21 +871,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -900,11 +900,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -926,9 +939,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -962,7 +977,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -971,136 +986,136 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1425,10 +1440,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D203"/>
+  <dimension ref="A1:D210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="A211" sqref="A211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="3"/>
@@ -1700,19 +1715,16 @@
       <c r="B23" t="s">
         <v>30</v>
       </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
       <c r="D23">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -1726,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
         <v>33</v>
@@ -1740,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
@@ -1754,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -1768,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
         <v>36</v>
@@ -1782,10 +1794,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
       </c>
       <c r="D29">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1793,27 +1808,24 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1821,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
         <v>39</v>
@@ -1835,7 +1847,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
         <v>40</v>
@@ -1849,7 +1861,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
@@ -1863,7 +1875,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
         <v>42</v>
@@ -1877,10 +1889,13 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1888,27 +1903,24 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1916,7 +1928,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -1930,7 +1942,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
@@ -1944,7 +1956,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -1958,7 +1970,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
@@ -1972,10 +1984,13 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>48</v>
       </c>
       <c r="D43">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1983,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D44">
         <v>19</v>
@@ -1994,27 +2009,24 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2022,7 +2034,7 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C47" t="s">
         <v>49</v>
@@ -2036,7 +2048,7 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
         <v>50</v>
@@ -2050,7 +2062,7 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
         <v>51</v>
@@ -2064,7 +2076,7 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
         <v>52</v>
@@ -2078,10 +2090,13 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>53</v>
       </c>
       <c r="D51">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2089,27 +2104,24 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53">
         <v>4</v>
-      </c>
-      <c r="C53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2117,10 +2129,10 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2131,10 +2143,10 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2145,7 +2157,7 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
         <v>55</v>
@@ -2159,7 +2171,7 @@
         <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s">
         <v>56</v>
@@ -2173,10 +2185,13 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C58" t="s">
+        <v>57</v>
       </c>
       <c r="D58">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2184,10 +2199,7 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
-      </c>
-      <c r="C59" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D59">
         <v>5</v>
@@ -2195,16 +2207,16 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2212,7 +2224,7 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C61" t="s">
         <v>58</v>
@@ -2226,7 +2238,7 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
         <v>59</v>
@@ -2240,7 +2252,7 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
         <v>60</v>
@@ -2254,7 +2266,7 @@
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
         <v>61</v>
@@ -2268,10 +2280,13 @@
         <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C65" t="s">
+        <v>62</v>
       </c>
       <c r="D65">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2279,10 +2294,10 @@
         <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D66">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2290,13 +2305,10 @@
         <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
-      </c>
-      <c r="C67" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D67">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2304,24 +2316,24 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
       </c>
       <c r="D68">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2329,7 +2341,7 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
         <v>63</v>
@@ -2343,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
         <v>64</v>
@@ -2357,7 +2369,7 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C72" t="s">
         <v>65</v>
@@ -2371,7 +2383,7 @@
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C73" t="s">
         <v>66</v>
@@ -2385,10 +2397,13 @@
         <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C74" t="s">
+        <v>67</v>
       </c>
       <c r="D74">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2396,10 +2411,10 @@
         <v>7</v>
       </c>
       <c r="B75" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75">
         <v>23</v>
-      </c>
-      <c r="D75">
-        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2407,24 +2422,24 @@
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>20</v>
-      </c>
-      <c r="C76" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D76">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="C77" t="s">
+        <v>38</v>
       </c>
       <c r="D77">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2432,27 +2447,24 @@
         <v>8</v>
       </c>
       <c r="B78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78">
         <v>21</v>
-      </c>
-      <c r="C78" t="s">
-        <v>37</v>
-      </c>
-      <c r="D78">
-        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2460,7 +2472,7 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C80" t="s">
         <v>68</v>
@@ -2474,7 +2486,7 @@
         <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
         <v>69</v>
@@ -2488,7 +2500,7 @@
         <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C82" t="s">
         <v>70</v>
@@ -2502,7 +2514,7 @@
         <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C83" t="s">
         <v>71</v>
@@ -2516,10 +2528,13 @@
         <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C84" t="s">
+        <v>72</v>
       </c>
       <c r="D84">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2527,13 +2542,10 @@
         <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>22</v>
-      </c>
-      <c r="C85" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2541,13 +2553,13 @@
         <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2555,13 +2567,13 @@
         <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C87" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D87">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2569,13 +2581,13 @@
         <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C88" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2583,13 +2595,13 @@
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C89" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D89">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2597,13 +2609,13 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D90">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2611,13 +2623,13 @@
         <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C91" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D91">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2625,13 +2637,13 @@
         <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D92">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2639,13 +2651,13 @@
         <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C93" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D93">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2653,13 +2665,13 @@
         <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C94" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D94">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2667,13 +2679,13 @@
         <v>9</v>
       </c>
       <c r="B95" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C95" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D95">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2681,13 +2693,13 @@
         <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C96" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D96">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2695,13 +2707,13 @@
         <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C97" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D97">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2709,13 +2721,13 @@
         <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C98" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D98">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2723,27 +2735,27 @@
         <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C99" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D99">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C100" t="s">
         <v>73</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2751,7 +2763,7 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C101" t="s">
         <v>74</v>
@@ -2765,7 +2777,7 @@
         <v>10</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C102" t="s">
         <v>75</v>
@@ -2779,7 +2791,7 @@
         <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C103" t="s">
         <v>76</v>
@@ -2793,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C104" t="s">
         <v>77</v>
@@ -2807,10 +2819,13 @@
         <v>10</v>
       </c>
       <c r="B105" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C105" t="s">
+        <v>78</v>
       </c>
       <c r="D105">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2818,27 +2833,24 @@
         <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>23</v>
-      </c>
-      <c r="C106" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D106">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C107" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2846,7 +2858,7 @@
         <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C108" t="s">
         <v>79</v>
@@ -2860,7 +2872,7 @@
         <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C109" t="s">
         <v>80</v>
@@ -2874,7 +2886,7 @@
         <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C110" t="s">
         <v>81</v>
@@ -2888,7 +2900,7 @@
         <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C111" t="s">
         <v>82</v>
@@ -2902,10 +2914,13 @@
         <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C112" t="s">
+        <v>83</v>
       </c>
       <c r="D112">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2913,27 +2928,24 @@
         <v>11</v>
       </c>
       <c r="B113" t="s">
-        <v>24</v>
-      </c>
-      <c r="C113" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D113">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C114" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2941,7 +2953,7 @@
         <v>12</v>
       </c>
       <c r="B115" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C115" t="s">
         <v>84</v>
@@ -2955,7 +2967,7 @@
         <v>12</v>
       </c>
       <c r="B116" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C116" t="s">
         <v>85</v>
@@ -2969,7 +2981,7 @@
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C117" t="s">
         <v>86</v>
@@ -2983,7 +2995,7 @@
         <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C118" t="s">
         <v>87</v>
@@ -2997,10 +3009,13 @@
         <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C119" t="s">
+        <v>88</v>
       </c>
       <c r="D119">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3008,27 +3023,24 @@
         <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
-      </c>
-      <c r="C120" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D120">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C121" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3036,7 +3048,7 @@
         <v>13</v>
       </c>
       <c r="B122" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C122" t="s">
         <v>89</v>
@@ -3050,7 +3062,7 @@
         <v>13</v>
       </c>
       <c r="B123" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C123" t="s">
         <v>90</v>
@@ -3064,7 +3076,7 @@
         <v>13</v>
       </c>
       <c r="B124" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C124" t="s">
         <v>91</v>
@@ -3078,7 +3090,7 @@
         <v>13</v>
       </c>
       <c r="B125" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C125" t="s">
         <v>92</v>
@@ -3092,10 +3104,13 @@
         <v>13</v>
       </c>
       <c r="B126" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C126" t="s">
+        <v>93</v>
       </c>
       <c r="D126">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3103,27 +3118,24 @@
         <v>13</v>
       </c>
       <c r="B127" t="s">
-        <v>26</v>
-      </c>
-      <c r="C127" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D127">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C128" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3131,7 +3143,7 @@
         <v>14</v>
       </c>
       <c r="B129" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C129" t="s">
         <v>94</v>
@@ -3145,7 +3157,7 @@
         <v>14</v>
       </c>
       <c r="B130" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C130" t="s">
         <v>95</v>
@@ -3159,7 +3171,7 @@
         <v>14</v>
       </c>
       <c r="B131" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C131" t="s">
         <v>96</v>
@@ -3170,10 +3182,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C132" t="s">
         <v>97</v>
@@ -3187,7 +3199,7 @@
         <v>15</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C133" t="s">
         <v>98</v>
@@ -3201,7 +3213,7 @@
         <v>15</v>
       </c>
       <c r="B134" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C134" t="s">
         <v>99</v>
@@ -3215,7 +3227,7 @@
         <v>15</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C135" t="s">
         <v>100</v>
@@ -3229,7 +3241,7 @@
         <v>15</v>
       </c>
       <c r="B136" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C136" t="s">
         <v>101</v>
@@ -3243,10 +3255,13 @@
         <v>15</v>
       </c>
       <c r="B137" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C137" t="s">
+        <v>102</v>
       </c>
       <c r="D137">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3254,27 +3269,24 @@
         <v>15</v>
       </c>
       <c r="B138" t="s">
-        <v>28</v>
-      </c>
-      <c r="C138" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D138">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C139" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3282,7 +3294,7 @@
         <v>16</v>
       </c>
       <c r="B140" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C140" t="s">
         <v>103</v>
@@ -3296,10 +3308,10 @@
         <v>16</v>
       </c>
       <c r="B141" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -3310,10 +3322,10 @@
         <v>16</v>
       </c>
       <c r="B142" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C142" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -3324,7 +3336,7 @@
         <v>16</v>
       </c>
       <c r="B143" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C143" t="s">
         <v>105</v>
@@ -3335,10 +3347,10 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C144" t="s">
         <v>106</v>
@@ -3352,7 +3364,7 @@
         <v>17</v>
       </c>
       <c r="B145" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C145" t="s">
         <v>107</v>
@@ -3366,7 +3378,7 @@
         <v>17</v>
       </c>
       <c r="B146" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C146" t="s">
         <v>108</v>
@@ -3380,7 +3392,7 @@
         <v>17</v>
       </c>
       <c r="B147" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C147" t="s">
         <v>109</v>
@@ -3391,10 +3403,10 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B148" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C148" t="s">
         <v>110</v>
@@ -3408,7 +3420,7 @@
         <v>18</v>
       </c>
       <c r="B149" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C149" t="s">
         <v>111</v>
@@ -3422,7 +3434,7 @@
         <v>18</v>
       </c>
       <c r="B150" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C150" t="s">
         <v>112</v>
@@ -3436,7 +3448,7 @@
         <v>18</v>
       </c>
       <c r="B151" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C151" t="s">
         <v>113</v>
@@ -3447,10 +3459,10 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B152" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C152" t="s">
         <v>114</v>
@@ -3464,10 +3476,10 @@
         <v>19</v>
       </c>
       <c r="B153" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="D153">
         <v>0</v>
@@ -3478,10 +3490,10 @@
         <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -3492,7 +3504,7 @@
         <v>19</v>
       </c>
       <c r="B155" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C155" t="s">
         <v>116</v>
@@ -3506,7 +3518,7 @@
         <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C156" t="s">
         <v>117</v>
@@ -3517,13 +3529,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C157" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -3534,7 +3546,7 @@
         <v>20</v>
       </c>
       <c r="B158" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C158" t="s">
         <v>54</v>
@@ -3548,7 +3560,7 @@
         <v>20</v>
       </c>
       <c r="B159" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C159" t="s">
         <v>55</v>
@@ -3562,7 +3574,7 @@
         <v>20</v>
       </c>
       <c r="B160" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C160" t="s">
         <v>56</v>
@@ -3573,13 +3585,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B161" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C161" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -3590,10 +3602,10 @@
         <v>21</v>
       </c>
       <c r="B162" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D162">
         <v>0</v>
@@ -3604,10 +3616,10 @@
         <v>21</v>
       </c>
       <c r="B163" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C163" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -3618,7 +3630,7 @@
         <v>21</v>
       </c>
       <c r="B164" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C164" t="s">
         <v>120</v>
@@ -3632,7 +3644,7 @@
         <v>21</v>
       </c>
       <c r="B165" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C165" t="s">
         <v>121</v>
@@ -3643,10 +3655,10 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B166" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C166" t="s">
         <v>122</v>
@@ -3660,7 +3672,7 @@
         <v>22</v>
       </c>
       <c r="B167" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C167" t="s">
         <v>123</v>
@@ -3671,10 +3683,10 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B168" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C168" t="s">
         <v>124</v>
@@ -3688,7 +3700,7 @@
         <v>23</v>
       </c>
       <c r="B169" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C169" t="s">
         <v>125</v>
@@ -3702,7 +3714,7 @@
         <v>23</v>
       </c>
       <c r="B170" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C170" t="s">
         <v>126</v>
@@ -3716,7 +3728,7 @@
         <v>23</v>
       </c>
       <c r="B171" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C171" t="s">
         <v>127</v>
@@ -3727,10 +3739,10 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B172" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C172" t="s">
         <v>128</v>
@@ -3744,7 +3756,7 @@
         <v>24</v>
       </c>
       <c r="B173" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C173" t="s">
         <v>129</v>
@@ -3758,7 +3770,7 @@
         <v>24</v>
       </c>
       <c r="B174" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C174" t="s">
         <v>130</v>
@@ -3769,10 +3781,10 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B175" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C175" t="s">
         <v>131</v>
@@ -3786,7 +3798,7 @@
         <v>25</v>
       </c>
       <c r="B176" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C176" t="s">
         <v>132</v>
@@ -3800,7 +3812,7 @@
         <v>25</v>
       </c>
       <c r="B177" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C177" t="s">
         <v>133</v>
@@ -3814,7 +3826,7 @@
         <v>25</v>
       </c>
       <c r="B178" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C178" t="s">
         <v>134</v>
@@ -3825,10 +3837,10 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B179" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C179" t="s">
         <v>135</v>
@@ -3842,7 +3854,7 @@
         <v>26</v>
       </c>
       <c r="B180" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C180" t="s">
         <v>136</v>
@@ -3856,7 +3868,7 @@
         <v>26</v>
       </c>
       <c r="B181" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C181" t="s">
         <v>137</v>
@@ -3870,7 +3882,7 @@
         <v>26</v>
       </c>
       <c r="B182" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C182" t="s">
         <v>138</v>
@@ -3881,10 +3893,10 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B183" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C183" t="s">
         <v>139</v>
@@ -3898,7 +3910,7 @@
         <v>27</v>
       </c>
       <c r="B184" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C184" t="s">
         <v>140</v>
@@ -3912,7 +3924,7 @@
         <v>27</v>
       </c>
       <c r="B185" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C185" t="s">
         <v>141</v>
@@ -3926,7 +3938,7 @@
         <v>27</v>
       </c>
       <c r="B186" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C186" t="s">
         <v>142</v>
@@ -3937,10 +3949,10 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B187" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C187" t="s">
         <v>143</v>
@@ -3954,7 +3966,7 @@
         <v>28</v>
       </c>
       <c r="B188" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C188" t="s">
         <v>144</v>
@@ -3968,7 +3980,7 @@
         <v>28</v>
       </c>
       <c r="B189" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C189" t="s">
         <v>145</v>
@@ -3982,7 +3994,7 @@
         <v>28</v>
       </c>
       <c r="B190" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C190" t="s">
         <v>146</v>
@@ -3993,10 +4005,10 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B191" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C191" t="s">
         <v>147</v>
@@ -4010,7 +4022,7 @@
         <v>29</v>
       </c>
       <c r="B192" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C192" t="s">
         <v>148</v>
@@ -4024,7 +4036,7 @@
         <v>29</v>
       </c>
       <c r="B193" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C193" t="s">
         <v>149</v>
@@ -4038,7 +4050,7 @@
         <v>29</v>
       </c>
       <c r="B194" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C194" t="s">
         <v>150</v>
@@ -4049,10 +4061,10 @@
     </row>
     <row r="195" spans="1:4">
       <c r="A195">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B195" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C195" t="s">
         <v>151</v>
@@ -4066,7 +4078,7 @@
         <v>30</v>
       </c>
       <c r="B196" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C196" t="s">
         <v>152</v>
@@ -4080,7 +4092,7 @@
         <v>30</v>
       </c>
       <c r="B197" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C197" t="s">
         <v>153</v>
@@ -4094,7 +4106,7 @@
         <v>30</v>
       </c>
       <c r="B198" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C198" t="s">
         <v>154</v>
@@ -4105,10 +4117,10 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B199" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C199" t="s">
         <v>155</v>
@@ -4122,7 +4134,7 @@
         <v>31</v>
       </c>
       <c r="B200" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C200" t="s">
         <v>156</v>
@@ -4136,10 +4148,10 @@
         <v>31</v>
       </c>
       <c r="B201" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C201" t="s">
-        <v>59</v>
+        <v>157</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -4150,10 +4162,10 @@
         <v>31</v>
       </c>
       <c r="B202" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C202" t="s">
-        <v>157</v>
+        <v>60</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -4164,13 +4176,111 @@
         <v>31</v>
       </c>
       <c r="B203" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C203" t="s">
         <v>158</v>
       </c>
       <c r="D203">
         <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204">
+        <v>31</v>
+      </c>
+      <c r="B204" t="s">
+        <v>12</v>
+      </c>
+      <c r="C204" t="s">
+        <v>159</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205">
+        <v>32</v>
+      </c>
+      <c r="B205" t="s">
+        <v>4</v>
+      </c>
+      <c r="C205" t="s">
+        <v>160</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206">
+        <v>32</v>
+      </c>
+      <c r="B206" t="s">
+        <v>6</v>
+      </c>
+      <c r="C206" t="s">
+        <v>161</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207">
+        <v>32</v>
+      </c>
+      <c r="B207" t="s">
+        <v>8</v>
+      </c>
+      <c r="C207" t="s">
+        <v>76</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208">
+        <v>32</v>
+      </c>
+      <c r="B208" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208" t="s">
+        <v>162</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209">
+        <v>32</v>
+      </c>
+      <c r="B209" t="s">
+        <v>12</v>
+      </c>
+      <c r="C209" t="s">
+        <v>163</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210">
+        <v>32</v>
+      </c>
+      <c r="B210" t="s">
+        <v>30</v>
+      </c>
+      <c r="C210" t="s">
+        <v>38</v>
+      </c>
+      <c r="D210">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>